<commit_message>
Add plqy into kafka
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_ZnI.xlsx
+++ b/scripts/inputs_qserver_kafka_ZnI.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="68">
   <si>
     <t xml:space="preserve">Input parameters for tasks in queue and kafka</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t xml:space="preserve">distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLQY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quinine</t>
   </si>
   <si>
     <t xml:space="preserve">pump_list</t>
@@ -175,6 +181,9 @@
   </si>
   <si>
     <t xml:space="preserve">kwargs for scipy.signal.find_peaks in _data_analysis.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If calculate plqy, reference name, excitation wavelength, absorbance_reference, PL_integral_reference, refractive_index_reference, plqy_reference</t>
   </si>
   <si>
     <t xml:space="preserve">dds1_p1, dd1_p2, dds2_p1, dds2_p2</t>
@@ -342,12 +351,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,10 +389,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -466,41 +479,53 @@
       <c r="A7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>10</v>
+      <c r="D7" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.37639</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>468573</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1.337</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.546</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -508,73 +533,70 @@
       <c r="A10" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>50</v>
+      <c r="B10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>19</v>
+      <c r="B11" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>24</v>
+      <c r="C12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,96 +604,99 @@
         <v>30</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0.5</v>
+        <v>50</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="B16" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>32</v>
+      <c r="B17" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="0" t="n">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D21" s="0" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>0</v>
@@ -685,7 +710,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>0</v>
@@ -694,6 +719,20 @@
         <v>0</v>
       </c>
       <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -713,10 +752,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -731,8 +770,8 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>38</v>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,65 +779,63 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>40</v>
+      <c r="B3" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>41</v>
+      <c r="B4" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>42</v>
+      <c r="B5" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>42</v>
+      <c r="B6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>43</v>
+      <c r="B7" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -807,43 +844,45 @@
       <c r="A10" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="B10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>49</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,61 +890,69 @@
         <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>31</v>
+      <c r="A17" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>54</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>55</v>
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="A20" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -924,10 +971,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -956,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,70 +1061,82 @@
       <c r="A7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>10</v>
+      <c r="D7" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.37639</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>468573</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1.337</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.546</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>61</v>
+      <c r="D8" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>50</v>
+      <c r="B10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>19</v>
+      <c r="B11" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,38 +1144,35 @@
         <v>20</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>27</v>
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>300</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1124,96 +1180,99 @@
         <v>30</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>4</v>
+        <v>50</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="B16" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>32</v>
+      <c r="B17" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>32</v>
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>32</v>
+      <c r="A19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="0" t="n">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D21" s="0" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>0</v>
@@ -1227,7 +1286,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>0</v>
@@ -1236,6 +1295,20 @@
         <v>0</v>
       </c>
       <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>